<commit_message>
[WIP] transfort rightsEnd into daterange
</commit_message>
<xml_diff>
--- a/libs/shared-assets/templates/import-movie-template.xlsx
+++ b/libs/shared-assets/templates/import-movie-template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="425">
   <si>
     <t xml:space="preserve">Film Library Metadata</t>
   </si>
@@ -115,6 +115,10 @@
   <si>
     <t xml:space="preserve">Scoring
 (A, B, C, D)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandate Beginning of rights 
+(MM/DD/YYYY)</t>
   </si>
   <si>
     <t xml:space="preserve">Mandate End of rights 
@@ -1730,33 +1734,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="38.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="31.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="20" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="26.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="25" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="29.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="33" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="34.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="38.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="31.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="26.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="34" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="37" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1795,42 +1799,42 @@
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="T8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X8" s="7" t="s">
+      <c r="Y8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7" t="s">
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="5"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="AB9" s="9"/>
+      <c r="H9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="Y9" s="8"/>
       <c r="AC9" s="9"/>
       <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
@@ -1860,7 +1864,7 @@
       <c r="I10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="K10" s="12" t="s">
@@ -1875,16 +1879,16 @@
       <c r="N10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="13" t="s">
+      <c r="O10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="R10" s="12" t="s">
+      <c r="R10" s="13" t="s">
         <v>29</v>
       </c>
       <c r="S10" s="12" t="s">
@@ -1922,31 +1926,34 @@
       </c>
       <c r="AD10" s="12" t="s">
         <v>41</v>
+      </c>
+      <c r="AE10" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B2"/>
-    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="AC9:AE9"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F9 P9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G9 Q9" type="list">
       <formula1>'Pre-defined lists'!$C$2:$C$256</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H9" type="list">
       <formula1>'Pre-defined lists'!$B$2:$B$21</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T9" type="list">
       <formula1>'Pre-defined lists'!$D$2:$D$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y9" type="list">
       <formula1>'Pre-defined lists'!$A$2:$A$19</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC9" type="list">
       <formula1>'Pre-defined lists'!$E$2:$E$83</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1983,990 +1990,990 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="20" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="20"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="20" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20"/>
       <c r="B45" s="20"/>
       <c r="C45" s="20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="20"/>
       <c r="B46" s="20"/>
       <c r="C46" s="20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="20"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20"/>
       <c r="B48" s="20"/>
       <c r="C48" s="20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="20"/>
       <c r="B51" s="20"/>
       <c r="C51" s="20" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="20" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="20" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="20" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="20" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="C57" s="20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D59" s="19"/>
       <c r="E59" s="20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="C60" s="20" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D60" s="19"/>
       <c r="E60" s="20" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="C61" s="20" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="20"/>
       <c r="B62" s="20"/>
       <c r="C62" s="20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
       <c r="C63" s="20" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D63" s="19"/>
       <c r="E63" s="20" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
       <c r="C64" s="20" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D64" s="19"/>
       <c r="E64" s="20" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="20" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D65" s="19"/>
       <c r="E65" s="20" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="20"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="20" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="C67" s="20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="20"/>
       <c r="B68" s="20"/>
       <c r="C68" s="20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D68" s="19"/>
       <c r="E68" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="20"/>
       <c r="B69" s="20"/>
       <c r="C69" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D69" s="19"/>
       <c r="E69" s="20" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="20"/>
       <c r="B70" s="20"/>
       <c r="C70" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D70" s="19"/>
       <c r="E70" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="20"/>
       <c r="B71" s="20"/>
       <c r="C71" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D71" s="19"/>
       <c r="E71" s="20" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
       <c r="C72" s="20" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D72" s="19"/>
       <c r="E72" s="20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
       <c r="C73" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
       <c r="C74" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D74" s="19"/>
       <c r="E74" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="C75" s="20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D75" s="19"/>
       <c r="E75" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
       <c r="C76" s="20" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D76" s="19"/>
       <c r="E76" s="20" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="C77" s="20" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D77" s="19"/>
       <c r="E77" s="20" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
       <c r="C78" s="20" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D78" s="19"/>
       <c r="E78" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
       <c r="C79" s="20" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D79" s="19"/>
       <c r="E79" s="20" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="20"/>
       <c r="B80" s="20"/>
       <c r="C80" s="20" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D80" s="19"/>
       <c r="E80" s="20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="20"/>
       <c r="B81" s="20"/>
       <c r="C81" s="20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D81" s="19"/>
       <c r="E81" s="20" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="C82" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D82" s="19"/>
       <c r="E82" s="20" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
       <c r="C83" s="20" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D83" s="19"/>
       <c r="E83" s="20" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
       <c r="C84" s="20" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D84" s="19"/>
       <c r="E84" s="20"/>
@@ -2975,7 +2982,7 @@
       <c r="A85" s="20"/>
       <c r="B85" s="20"/>
       <c r="C85" s="20" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D85" s="19"/>
       <c r="E85" s="20"/>
@@ -2984,7 +2991,7 @@
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
       <c r="C86" s="20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D86" s="19"/>
       <c r="E86" s="20"/>
@@ -2993,7 +3000,7 @@
       <c r="A87" s="20"/>
       <c r="B87" s="20"/>
       <c r="C87" s="20" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D87" s="19"/>
       <c r="E87" s="20"/>
@@ -3002,7 +3009,7 @@
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="C88" s="20" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="20"/>
@@ -3011,7 +3018,7 @@
       <c r="A89" s="20"/>
       <c r="B89" s="20"/>
       <c r="C89" s="20" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D89" s="19"/>
       <c r="E89" s="20"/>
@@ -3020,7 +3027,7 @@
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="C90" s="20" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D90" s="19"/>
       <c r="E90" s="20"/>
@@ -3029,7 +3036,7 @@
       <c r="A91" s="20"/>
       <c r="B91" s="20"/>
       <c r="C91" s="20" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D91" s="19"/>
       <c r="E91" s="20"/>
@@ -3038,7 +3045,7 @@
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="C92" s="20" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D92" s="19"/>
       <c r="E92" s="20"/>
@@ -3047,7 +3054,7 @@
       <c r="A93" s="20"/>
       <c r="B93" s="20"/>
       <c r="C93" s="20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D93" s="19"/>
       <c r="E93" s="20"/>
@@ -3056,7 +3063,7 @@
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="C94" s="20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D94" s="19"/>
       <c r="E94" s="20"/>
@@ -3065,7 +3072,7 @@
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="C95" s="20" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D95" s="19"/>
       <c r="E95" s="20"/>
@@ -3074,7 +3081,7 @@
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="C96" s="20" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D96" s="19"/>
       <c r="E96" s="20"/>
@@ -3083,7 +3090,7 @@
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="C97" s="20" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="20"/>
@@ -3092,7 +3099,7 @@
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="C98" s="20" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D98" s="19"/>
       <c r="E98" s="20"/>
@@ -3101,7 +3108,7 @@
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="C99" s="20" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D99" s="19"/>
       <c r="E99" s="20"/>
@@ -3110,7 +3117,7 @@
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="C100" s="20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D100" s="19"/>
       <c r="E100" s="20"/>
@@ -3119,7 +3126,7 @@
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="C101" s="20" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D101" s="19"/>
       <c r="E101" s="20"/>
@@ -3128,7 +3135,7 @@
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="C102" s="20" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="20"/>
@@ -3137,7 +3144,7 @@
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="C103" s="20" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D103" s="19"/>
       <c r="E103" s="20"/>
@@ -3146,7 +3153,7 @@
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
       <c r="C104" s="20" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D104" s="19"/>
       <c r="E104" s="20"/>
@@ -3155,7 +3162,7 @@
       <c r="A105" s="20"/>
       <c r="B105" s="20"/>
       <c r="C105" s="20" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D105" s="19"/>
       <c r="E105" s="20"/>
@@ -3164,7 +3171,7 @@
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="C106" s="20" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D106" s="19"/>
       <c r="E106" s="20"/>
@@ -3173,7 +3180,7 @@
       <c r="A107" s="20"/>
       <c r="B107" s="20"/>
       <c r="C107" s="20" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D107" s="19"/>
       <c r="E107" s="20"/>
@@ -3182,7 +3189,7 @@
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
       <c r="C108" s="20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D108" s="19"/>
       <c r="E108" s="20"/>
@@ -3191,7 +3198,7 @@
       <c r="A109" s="20"/>
       <c r="B109" s="20"/>
       <c r="C109" s="20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D109" s="19"/>
       <c r="E109" s="20"/>
@@ -3200,7 +3207,7 @@
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="C110" s="20" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D110" s="19"/>
       <c r="E110" s="20"/>
@@ -3209,7 +3216,7 @@
       <c r="A111" s="20"/>
       <c r="B111" s="20"/>
       <c r="C111" s="20" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D111" s="19"/>
       <c r="E111" s="20"/>
@@ -3218,7 +3225,7 @@
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
       <c r="C112" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D112" s="19"/>
       <c r="E112" s="20"/>
@@ -3227,7 +3234,7 @@
       <c r="A113" s="20"/>
       <c r="B113" s="20"/>
       <c r="C113" s="20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D113" s="19"/>
       <c r="E113" s="20"/>
@@ -3236,7 +3243,7 @@
       <c r="A114" s="20"/>
       <c r="B114" s="20"/>
       <c r="C114" s="20" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D114" s="19"/>
       <c r="E114" s="20"/>
@@ -3245,7 +3252,7 @@
       <c r="A115" s="20"/>
       <c r="B115" s="20"/>
       <c r="C115" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D115" s="19"/>
       <c r="E115" s="20"/>
@@ -3254,7 +3261,7 @@
       <c r="A116" s="20"/>
       <c r="B116" s="20"/>
       <c r="C116" s="20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D116" s="19"/>
       <c r="E116" s="20"/>
@@ -3263,7 +3270,7 @@
       <c r="A117" s="20"/>
       <c r="B117" s="20"/>
       <c r="C117" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D117" s="19"/>
       <c r="E117" s="20"/>
@@ -3272,7 +3279,7 @@
       <c r="A118" s="20"/>
       <c r="B118" s="20"/>
       <c r="C118" s="20" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D118" s="19"/>
       <c r="E118" s="20"/>
@@ -3281,7 +3288,7 @@
       <c r="A119" s="20"/>
       <c r="B119" s="20"/>
       <c r="C119" s="20" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D119" s="19"/>
       <c r="E119" s="20"/>
@@ -3290,7 +3297,7 @@
       <c r="A120" s="20"/>
       <c r="B120" s="20"/>
       <c r="C120" s="20" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D120" s="19"/>
       <c r="E120" s="20"/>
@@ -3299,7 +3306,7 @@
       <c r="A121" s="20"/>
       <c r="B121" s="20"/>
       <c r="C121" s="20" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D121" s="19"/>
       <c r="E121" s="20"/>
@@ -3308,7 +3315,7 @@
       <c r="A122" s="20"/>
       <c r="B122" s="20"/>
       <c r="C122" s="20" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D122" s="19"/>
       <c r="E122" s="20"/>
@@ -3317,7 +3324,7 @@
       <c r="A123" s="20"/>
       <c r="B123" s="20"/>
       <c r="C123" s="20" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D123" s="19"/>
       <c r="E123" s="20"/>
@@ -3326,7 +3333,7 @@
       <c r="A124" s="20"/>
       <c r="B124" s="20"/>
       <c r="C124" s="20" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D124" s="19"/>
       <c r="E124" s="20"/>
@@ -3335,7 +3342,7 @@
       <c r="A125" s="20"/>
       <c r="B125" s="20"/>
       <c r="C125" s="20" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D125" s="19"/>
       <c r="E125" s="20"/>
@@ -3344,7 +3351,7 @@
       <c r="A126" s="20"/>
       <c r="B126" s="20"/>
       <c r="C126" s="20" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D126" s="19"/>
       <c r="E126" s="20"/>
@@ -3353,7 +3360,7 @@
       <c r="A127" s="20"/>
       <c r="B127" s="20"/>
       <c r="C127" s="20" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D127" s="19"/>
       <c r="E127" s="20"/>
@@ -3362,7 +3369,7 @@
       <c r="A128" s="20"/>
       <c r="B128" s="20"/>
       <c r="C128" s="20" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D128" s="19"/>
       <c r="E128" s="20"/>
@@ -3371,7 +3378,7 @@
       <c r="A129" s="20"/>
       <c r="B129" s="20"/>
       <c r="C129" s="20" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D129" s="19"/>
       <c r="E129" s="20"/>
@@ -3380,7 +3387,7 @@
       <c r="A130" s="20"/>
       <c r="B130" s="20"/>
       <c r="C130" s="20" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D130" s="19"/>
       <c r="E130" s="20"/>
@@ -3389,7 +3396,7 @@
       <c r="A131" s="20"/>
       <c r="B131" s="20"/>
       <c r="C131" s="20" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D131" s="19"/>
       <c r="E131" s="20"/>
@@ -3398,7 +3405,7 @@
       <c r="A132" s="20"/>
       <c r="B132" s="20"/>
       <c r="C132" s="20" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D132" s="19"/>
       <c r="E132" s="20"/>
@@ -3407,7 +3414,7 @@
       <c r="A133" s="20"/>
       <c r="B133" s="20"/>
       <c r="C133" s="20" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D133" s="19"/>
       <c r="E133" s="20"/>
@@ -3416,7 +3423,7 @@
       <c r="A134" s="20"/>
       <c r="B134" s="20"/>
       <c r="C134" s="20" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D134" s="19"/>
       <c r="E134" s="20"/>
@@ -3425,7 +3432,7 @@
       <c r="A135" s="20"/>
       <c r="B135" s="20"/>
       <c r="C135" s="20" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D135" s="19"/>
       <c r="E135" s="20"/>
@@ -3434,7 +3441,7 @@
       <c r="A136" s="20"/>
       <c r="B136" s="20"/>
       <c r="C136" s="20" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D136" s="19"/>
       <c r="E136" s="20"/>
@@ -3443,7 +3450,7 @@
       <c r="A137" s="20"/>
       <c r="B137" s="20"/>
       <c r="C137" s="20" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D137" s="19"/>
       <c r="E137" s="20"/>
@@ -3452,7 +3459,7 @@
       <c r="A138" s="20"/>
       <c r="B138" s="20"/>
       <c r="C138" s="20" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D138" s="19"/>
       <c r="E138" s="20"/>
@@ -3461,7 +3468,7 @@
       <c r="A139" s="20"/>
       <c r="B139" s="20"/>
       <c r="C139" s="20" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D139" s="19"/>
       <c r="E139" s="20"/>
@@ -3470,7 +3477,7 @@
       <c r="A140" s="20"/>
       <c r="B140" s="20"/>
       <c r="C140" s="20" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D140" s="19"/>
       <c r="E140" s="20"/>
@@ -3479,7 +3486,7 @@
       <c r="A141" s="20"/>
       <c r="B141" s="20"/>
       <c r="C141" s="20" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D141" s="19"/>
       <c r="E141" s="20"/>
@@ -3488,7 +3495,7 @@
       <c r="A142" s="20"/>
       <c r="B142" s="20"/>
       <c r="C142" s="20" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D142" s="19"/>
       <c r="E142" s="20"/>
@@ -3497,7 +3504,7 @@
       <c r="A143" s="20"/>
       <c r="B143" s="20"/>
       <c r="C143" s="20" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D143" s="19"/>
       <c r="E143" s="20"/>
@@ -3506,7 +3513,7 @@
       <c r="A144" s="20"/>
       <c r="B144" s="20"/>
       <c r="C144" s="20" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D144" s="19"/>
       <c r="E144" s="20"/>
@@ -3515,7 +3522,7 @@
       <c r="A145" s="20"/>
       <c r="B145" s="20"/>
       <c r="C145" s="20" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D145" s="19"/>
       <c r="E145" s="20"/>
@@ -3524,7 +3531,7 @@
       <c r="A146" s="20"/>
       <c r="B146" s="20"/>
       <c r="C146" s="20" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D146" s="19"/>
       <c r="E146" s="20"/>
@@ -3533,7 +3540,7 @@
       <c r="A147" s="20"/>
       <c r="B147" s="20"/>
       <c r="C147" s="20" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D147" s="19"/>
       <c r="E147" s="20"/>
@@ -3542,7 +3549,7 @@
       <c r="A148" s="20"/>
       <c r="B148" s="20"/>
       <c r="C148" s="20" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D148" s="19"/>
       <c r="E148" s="20"/>
@@ -3551,7 +3558,7 @@
       <c r="A149" s="20"/>
       <c r="B149" s="20"/>
       <c r="C149" s="20" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D149" s="19"/>
       <c r="E149" s="20"/>
@@ -3560,7 +3567,7 @@
       <c r="A150" s="20"/>
       <c r="B150" s="20"/>
       <c r="C150" s="20" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D150" s="19"/>
       <c r="E150" s="20"/>
@@ -3569,7 +3576,7 @@
       <c r="A151" s="20"/>
       <c r="B151" s="20"/>
       <c r="C151" s="20" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D151" s="19"/>
       <c r="E151" s="20"/>
@@ -3578,7 +3585,7 @@
       <c r="A152" s="20"/>
       <c r="B152" s="20"/>
       <c r="C152" s="20" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D152" s="19"/>
       <c r="E152" s="20"/>
@@ -3587,7 +3594,7 @@
       <c r="A153" s="20"/>
       <c r="B153" s="20"/>
       <c r="C153" s="20" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D153" s="19"/>
       <c r="E153" s="20"/>
@@ -3596,7 +3603,7 @@
       <c r="A154" s="20"/>
       <c r="B154" s="20"/>
       <c r="C154" s="20" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D154" s="19"/>
       <c r="E154" s="20"/>
@@ -3605,7 +3612,7 @@
       <c r="A155" s="20"/>
       <c r="B155" s="20"/>
       <c r="C155" s="20" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D155" s="19"/>
       <c r="E155" s="20"/>
@@ -3614,7 +3621,7 @@
       <c r="A156" s="20"/>
       <c r="B156" s="20"/>
       <c r="C156" s="20" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D156" s="19"/>
       <c r="E156" s="20"/>
@@ -3623,7 +3630,7 @@
       <c r="A157" s="20"/>
       <c r="B157" s="20"/>
       <c r="C157" s="20" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D157" s="19"/>
       <c r="E157" s="20"/>
@@ -3632,7 +3639,7 @@
       <c r="A158" s="20"/>
       <c r="B158" s="20"/>
       <c r="C158" s="20" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D158" s="19"/>
       <c r="E158" s="20"/>
@@ -3641,7 +3648,7 @@
       <c r="A159" s="20"/>
       <c r="B159" s="20"/>
       <c r="C159" s="20" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D159" s="19"/>
       <c r="E159" s="20"/>
@@ -3650,7 +3657,7 @@
       <c r="A160" s="20"/>
       <c r="B160" s="20"/>
       <c r="C160" s="20" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D160" s="19"/>
       <c r="E160" s="20"/>
@@ -3659,7 +3666,7 @@
       <c r="A161" s="20"/>
       <c r="B161" s="20"/>
       <c r="C161" s="20" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D161" s="19"/>
       <c r="E161" s="20"/>
@@ -3668,7 +3675,7 @@
       <c r="A162" s="20"/>
       <c r="B162" s="20"/>
       <c r="C162" s="20" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D162" s="19"/>
       <c r="E162" s="20"/>
@@ -3677,7 +3684,7 @@
       <c r="A163" s="20"/>
       <c r="B163" s="20"/>
       <c r="C163" s="20" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D163" s="19"/>
       <c r="E163" s="20"/>
@@ -3686,7 +3693,7 @@
       <c r="A164" s="20"/>
       <c r="B164" s="20"/>
       <c r="C164" s="20" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="20"/>
@@ -3695,7 +3702,7 @@
       <c r="A165" s="20"/>
       <c r="B165" s="20"/>
       <c r="C165" s="20" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="20"/>
@@ -3704,7 +3711,7 @@
       <c r="A166" s="20"/>
       <c r="B166" s="20"/>
       <c r="C166" s="20" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="20"/>
@@ -3713,7 +3720,7 @@
       <c r="A167" s="20"/>
       <c r="B167" s="20"/>
       <c r="C167" s="20" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="20"/>
@@ -3722,7 +3729,7 @@
       <c r="A168" s="20"/>
       <c r="B168" s="20"/>
       <c r="C168" s="20" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="20"/>
@@ -3731,7 +3738,7 @@
       <c r="A169" s="20"/>
       <c r="B169" s="20"/>
       <c r="C169" s="20" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="20"/>
@@ -3740,7 +3747,7 @@
       <c r="A170" s="20"/>
       <c r="B170" s="20"/>
       <c r="C170" s="20" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="20"/>
@@ -3749,7 +3756,7 @@
       <c r="A171" s="20"/>
       <c r="B171" s="20"/>
       <c r="C171" s="20" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D171" s="19"/>
       <c r="E171" s="20"/>
@@ -3758,7 +3765,7 @@
       <c r="A172" s="20"/>
       <c r="B172" s="20"/>
       <c r="C172" s="20" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D172" s="19"/>
       <c r="E172" s="20"/>
@@ -3767,7 +3774,7 @@
       <c r="A173" s="20"/>
       <c r="B173" s="20"/>
       <c r="C173" s="20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D173" s="19"/>
       <c r="E173" s="20"/>
@@ -3776,7 +3783,7 @@
       <c r="A174" s="20"/>
       <c r="B174" s="20"/>
       <c r="C174" s="20" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D174" s="19"/>
       <c r="E174" s="20"/>
@@ -3785,7 +3792,7 @@
       <c r="A175" s="20"/>
       <c r="B175" s="20"/>
       <c r="C175" s="20" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D175" s="19"/>
       <c r="E175" s="20"/>
@@ -3794,7 +3801,7 @@
       <c r="A176" s="20"/>
       <c r="B176" s="20"/>
       <c r="C176" s="20" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D176" s="19"/>
       <c r="E176" s="20"/>
@@ -3803,7 +3810,7 @@
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="20" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D177" s="19"/>
       <c r="E177" s="20"/>
@@ -3812,7 +3819,7 @@
       <c r="A178" s="20"/>
       <c r="B178" s="20"/>
       <c r="C178" s="20" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D178" s="19"/>
       <c r="E178" s="20"/>
@@ -3821,7 +3828,7 @@
       <c r="A179" s="20"/>
       <c r="B179" s="20"/>
       <c r="C179" s="20" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D179" s="19"/>
       <c r="E179" s="20"/>
@@ -3830,7 +3837,7 @@
       <c r="A180" s="20"/>
       <c r="B180" s="20"/>
       <c r="C180" s="20" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D180" s="19"/>
       <c r="E180" s="20"/>
@@ -3839,7 +3846,7 @@
       <c r="A181" s="20"/>
       <c r="B181" s="20"/>
       <c r="C181" s="20" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D181" s="19"/>
       <c r="E181" s="20"/>
@@ -3848,7 +3855,7 @@
       <c r="A182" s="20"/>
       <c r="B182" s="20"/>
       <c r="C182" s="20" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D182" s="19"/>
       <c r="E182" s="20"/>
@@ -3857,7 +3864,7 @@
       <c r="A183" s="20"/>
       <c r="B183" s="20"/>
       <c r="C183" s="20" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D183" s="19"/>
       <c r="E183" s="20"/>
@@ -3866,7 +3873,7 @@
       <c r="A184" s="20"/>
       <c r="B184" s="20"/>
       <c r="C184" s="20" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D184" s="19"/>
       <c r="E184" s="20"/>
@@ -3875,7 +3882,7 @@
       <c r="A185" s="20"/>
       <c r="B185" s="20"/>
       <c r="C185" s="20" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D185" s="19"/>
       <c r="E185" s="20"/>
@@ -3884,7 +3891,7 @@
       <c r="A186" s="20"/>
       <c r="B186" s="20"/>
       <c r="C186" s="20" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D186" s="19"/>
       <c r="E186" s="20"/>
@@ -3893,7 +3900,7 @@
       <c r="A187" s="20"/>
       <c r="B187" s="20"/>
       <c r="C187" s="20" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D187" s="19"/>
       <c r="E187" s="20"/>
@@ -3902,7 +3909,7 @@
       <c r="A188" s="20"/>
       <c r="B188" s="20"/>
       <c r="C188" s="20" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D188" s="19"/>
       <c r="E188" s="20"/>
@@ -3911,7 +3918,7 @@
       <c r="A189" s="20"/>
       <c r="B189" s="20"/>
       <c r="C189" s="20" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D189" s="19"/>
       <c r="E189" s="20"/>
@@ -3920,7 +3927,7 @@
       <c r="A190" s="20"/>
       <c r="B190" s="20"/>
       <c r="C190" s="20" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D190" s="19"/>
       <c r="E190" s="20"/>
@@ -3929,7 +3936,7 @@
       <c r="A191" s="20"/>
       <c r="B191" s="20"/>
       <c r="C191" s="20" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D191" s="19"/>
       <c r="E191" s="20"/>
@@ -3938,7 +3945,7 @@
       <c r="A192" s="20"/>
       <c r="B192" s="20"/>
       <c r="C192" s="20" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D192" s="19"/>
       <c r="E192" s="20"/>
@@ -3947,7 +3954,7 @@
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
       <c r="C193" s="20" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D193" s="19"/>
       <c r="E193" s="20"/>
@@ -3956,7 +3963,7 @@
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
       <c r="C194" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D194" s="19"/>
       <c r="E194" s="20"/>
@@ -3965,7 +3972,7 @@
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
       <c r="C195" s="20" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D195" s="19"/>
       <c r="E195" s="20"/>
@@ -3974,7 +3981,7 @@
       <c r="A196" s="20"/>
       <c r="B196" s="20"/>
       <c r="C196" s="20" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D196" s="19"/>
       <c r="E196" s="20"/>
@@ -3983,7 +3990,7 @@
       <c r="A197" s="20"/>
       <c r="B197" s="20"/>
       <c r="C197" s="20" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D197" s="19"/>
       <c r="E197" s="20"/>
@@ -3992,7 +3999,7 @@
       <c r="A198" s="20"/>
       <c r="B198" s="20"/>
       <c r="C198" s="20" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D198" s="19"/>
       <c r="E198" s="20"/>
@@ -4001,7 +4008,7 @@
       <c r="A199" s="20"/>
       <c r="B199" s="20"/>
       <c r="C199" s="20" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D199" s="19"/>
       <c r="E199" s="20"/>
@@ -4010,7 +4017,7 @@
       <c r="A200" s="20"/>
       <c r="B200" s="20"/>
       <c r="C200" s="20" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D200" s="19"/>
       <c r="E200" s="20"/>
@@ -4019,7 +4026,7 @@
       <c r="A201" s="20"/>
       <c r="B201" s="20"/>
       <c r="C201" s="20" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D201" s="19"/>
       <c r="E201" s="20"/>
@@ -4028,7 +4035,7 @@
       <c r="A202" s="20"/>
       <c r="B202" s="20"/>
       <c r="C202" s="20" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D202" s="19"/>
       <c r="E202" s="20"/>
@@ -4037,7 +4044,7 @@
       <c r="A203" s="20"/>
       <c r="B203" s="20"/>
       <c r="C203" s="20" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D203" s="19"/>
       <c r="E203" s="20"/>
@@ -4046,7 +4053,7 @@
       <c r="A204" s="20"/>
       <c r="B204" s="20"/>
       <c r="C204" s="20" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D204" s="19"/>
       <c r="E204" s="20"/>
@@ -4055,7 +4062,7 @@
       <c r="A205" s="20"/>
       <c r="B205" s="20"/>
       <c r="C205" s="20" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D205" s="19"/>
       <c r="E205" s="20"/>
@@ -4064,7 +4071,7 @@
       <c r="A206" s="20"/>
       <c r="B206" s="20"/>
       <c r="C206" s="20" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D206" s="19"/>
       <c r="E206" s="20"/>
@@ -4073,7 +4080,7 @@
       <c r="A207" s="20"/>
       <c r="B207" s="20"/>
       <c r="C207" s="20" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D207" s="19"/>
       <c r="E207" s="20"/>
@@ -4082,7 +4089,7 @@
       <c r="A208" s="20"/>
       <c r="B208" s="20"/>
       <c r="C208" s="20" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D208" s="19"/>
       <c r="E208" s="20"/>
@@ -4091,7 +4098,7 @@
       <c r="A209" s="20"/>
       <c r="B209" s="20"/>
       <c r="C209" s="20" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D209" s="19"/>
       <c r="E209" s="20"/>
@@ -4100,7 +4107,7 @@
       <c r="A210" s="20"/>
       <c r="B210" s="20"/>
       <c r="C210" s="20" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D210" s="19"/>
       <c r="E210" s="20"/>
@@ -4109,7 +4116,7 @@
       <c r="A211" s="20"/>
       <c r="B211" s="20"/>
       <c r="C211" s="20" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D211" s="19"/>
       <c r="E211" s="20"/>
@@ -4118,7 +4125,7 @@
       <c r="A212" s="20"/>
       <c r="B212" s="20"/>
       <c r="C212" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D212" s="19"/>
       <c r="E212" s="20"/>
@@ -4127,7 +4134,7 @@
       <c r="A213" s="20"/>
       <c r="B213" s="20"/>
       <c r="C213" s="20" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D213" s="19"/>
       <c r="E213" s="20"/>
@@ -4136,7 +4143,7 @@
       <c r="A214" s="20"/>
       <c r="B214" s="20"/>
       <c r="C214" s="20" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D214" s="19"/>
       <c r="E214" s="20"/>
@@ -4145,7 +4152,7 @@
       <c r="A215" s="20"/>
       <c r="B215" s="20"/>
       <c r="C215" s="20" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D215" s="19"/>
       <c r="E215" s="20"/>
@@ -4154,7 +4161,7 @@
       <c r="A216" s="20"/>
       <c r="B216" s="20"/>
       <c r="C216" s="20" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D216" s="19"/>
       <c r="E216" s="20"/>
@@ -4163,7 +4170,7 @@
       <c r="A217" s="20"/>
       <c r="B217" s="20"/>
       <c r="C217" s="20" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D217" s="19"/>
       <c r="E217" s="20"/>
@@ -4172,7 +4179,7 @@
       <c r="A218" s="20"/>
       <c r="B218" s="20"/>
       <c r="C218" s="20" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D218" s="19"/>
       <c r="E218" s="20"/>
@@ -4181,7 +4188,7 @@
       <c r="A219" s="20"/>
       <c r="B219" s="20"/>
       <c r="C219" s="20" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D219" s="19"/>
       <c r="E219" s="20"/>
@@ -4190,7 +4197,7 @@
       <c r="A220" s="20"/>
       <c r="B220" s="20"/>
       <c r="C220" s="20" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D220" s="19"/>
       <c r="E220" s="20"/>
@@ -4199,7 +4206,7 @@
       <c r="A221" s="20"/>
       <c r="B221" s="20"/>
       <c r="C221" s="20" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D221" s="19"/>
       <c r="E221" s="20"/>
@@ -4208,7 +4215,7 @@
       <c r="A222" s="20"/>
       <c r="B222" s="20"/>
       <c r="C222" s="20" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D222" s="19"/>
       <c r="E222" s="20"/>
@@ -4217,7 +4224,7 @@
       <c r="A223" s="20"/>
       <c r="B223" s="20"/>
       <c r="C223" s="20" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D223" s="19"/>
       <c r="E223" s="20"/>
@@ -4226,7 +4233,7 @@
       <c r="A224" s="20"/>
       <c r="B224" s="20"/>
       <c r="C224" s="20" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D224" s="19"/>
       <c r="E224" s="20"/>
@@ -4235,7 +4242,7 @@
       <c r="A225" s="20"/>
       <c r="B225" s="20"/>
       <c r="C225" s="20" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D225" s="19"/>
       <c r="E225" s="20"/>
@@ -4244,7 +4251,7 @@
       <c r="A226" s="20"/>
       <c r="B226" s="20"/>
       <c r="C226" s="20" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D226" s="19"/>
       <c r="E226" s="20"/>
@@ -4253,7 +4260,7 @@
       <c r="A227" s="20"/>
       <c r="B227" s="20"/>
       <c r="C227" s="20" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D227" s="19"/>
       <c r="E227" s="20"/>
@@ -4262,7 +4269,7 @@
       <c r="A228" s="20"/>
       <c r="B228" s="20"/>
       <c r="C228" s="20" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D228" s="19"/>
       <c r="E228" s="20"/>
@@ -4271,7 +4278,7 @@
       <c r="A229" s="20"/>
       <c r="B229" s="20"/>
       <c r="C229" s="20" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D229" s="19"/>
       <c r="E229" s="20"/>
@@ -4280,7 +4287,7 @@
       <c r="A230" s="20"/>
       <c r="B230" s="20"/>
       <c r="C230" s="20" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D230" s="19"/>
       <c r="E230" s="20"/>
@@ -4289,7 +4296,7 @@
       <c r="A231" s="20"/>
       <c r="B231" s="20"/>
       <c r="C231" s="20" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D231" s="19"/>
       <c r="E231" s="20"/>
@@ -4298,7 +4305,7 @@
       <c r="A232" s="20"/>
       <c r="B232" s="20"/>
       <c r="C232" s="20" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D232" s="19"/>
       <c r="E232" s="20"/>
@@ -4307,7 +4314,7 @@
       <c r="A233" s="20"/>
       <c r="B233" s="20"/>
       <c r="C233" s="20" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D233" s="19"/>
       <c r="E233" s="20"/>
@@ -4316,7 +4323,7 @@
       <c r="A234" s="20"/>
       <c r="B234" s="20"/>
       <c r="C234" s="20" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D234" s="19"/>
       <c r="E234" s="20"/>
@@ -4325,7 +4332,7 @@
       <c r="A235" s="20"/>
       <c r="B235" s="20"/>
       <c r="C235" s="20" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D235" s="19"/>
       <c r="E235" s="20"/>
@@ -4334,7 +4341,7 @@
       <c r="A236" s="20"/>
       <c r="B236" s="20"/>
       <c r="C236" s="20" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D236" s="19"/>
       <c r="E236" s="20"/>
@@ -4343,7 +4350,7 @@
       <c r="A237" s="20"/>
       <c r="B237" s="20"/>
       <c r="C237" s="20" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D237" s="19"/>
       <c r="E237" s="20"/>
@@ -4352,7 +4359,7 @@
       <c r="A238" s="20"/>
       <c r="B238" s="20"/>
       <c r="C238" s="20" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D238" s="19"/>
       <c r="E238" s="20"/>
@@ -4361,7 +4368,7 @@
       <c r="A239" s="20"/>
       <c r="B239" s="20"/>
       <c r="C239" s="20" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D239" s="19"/>
       <c r="E239" s="20"/>
@@ -4370,7 +4377,7 @@
       <c r="A240" s="20"/>
       <c r="B240" s="20"/>
       <c r="C240" s="20" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D240" s="19"/>
       <c r="E240" s="20"/>
@@ -4379,7 +4386,7 @@
       <c r="A241" s="20"/>
       <c r="B241" s="20"/>
       <c r="C241" s="20" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D241" s="19"/>
       <c r="E241" s="20"/>
@@ -4388,7 +4395,7 @@
       <c r="A242" s="20"/>
       <c r="B242" s="20"/>
       <c r="C242" s="20" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D242" s="19"/>
       <c r="E242" s="20"/>
@@ -4397,7 +4404,7 @@
       <c r="A243" s="20"/>
       <c r="B243" s="20"/>
       <c r="C243" s="20" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D243" s="19"/>
       <c r="E243" s="20"/>
@@ -4406,7 +4413,7 @@
       <c r="A244" s="20"/>
       <c r="B244" s="20"/>
       <c r="C244" s="20" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D244" s="19"/>
       <c r="E244" s="20"/>
@@ -4415,7 +4422,7 @@
       <c r="A245" s="20"/>
       <c r="B245" s="20"/>
       <c r="C245" s="20" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D245" s="19"/>
       <c r="E245" s="20"/>
@@ -4424,7 +4431,7 @@
       <c r="A246" s="20"/>
       <c r="B246" s="20"/>
       <c r="C246" s="20" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D246" s="19"/>
       <c r="E246" s="20"/>
@@ -4433,7 +4440,7 @@
       <c r="A247" s="20"/>
       <c r="B247" s="20"/>
       <c r="C247" s="20" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D247" s="19"/>
       <c r="E247" s="20"/>
@@ -4442,7 +4449,7 @@
       <c r="A248" s="20"/>
       <c r="B248" s="20"/>
       <c r="C248" s="20" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D248" s="19"/>
       <c r="E248" s="20"/>
@@ -4451,7 +4458,7 @@
       <c r="A249" s="20"/>
       <c r="B249" s="20"/>
       <c r="C249" s="20" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D249" s="19"/>
       <c r="E249" s="20"/>
@@ -4460,7 +4467,7 @@
       <c r="A250" s="20"/>
       <c r="B250" s="20"/>
       <c r="C250" s="20" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D250" s="19"/>
       <c r="E250" s="20"/>
@@ -4469,7 +4476,7 @@
       <c r="A251" s="20"/>
       <c r="B251" s="20"/>
       <c r="C251" s="20" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D251" s="19"/>
       <c r="E251" s="20"/>
@@ -4478,7 +4485,7 @@
       <c r="A252" s="20"/>
       <c r="B252" s="20"/>
       <c r="C252" s="20" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D252" s="19"/>
       <c r="E252" s="20"/>
@@ -4487,7 +4494,7 @@
       <c r="A253" s="20"/>
       <c r="B253" s="20"/>
       <c r="C253" s="20" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D253" s="19"/>
       <c r="E253" s="20"/>
@@ -4496,7 +4503,7 @@
       <c r="A254" s="20"/>
       <c r="B254" s="20"/>
       <c r="C254" s="20" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D254" s="19"/>
       <c r="E254" s="20"/>
@@ -4505,7 +4512,7 @@
       <c r="A255" s="20"/>
       <c r="B255" s="20"/>
       <c r="C255" s="20" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D255" s="19"/>
       <c r="E255" s="20"/>
@@ -4514,7 +4521,7 @@
       <c r="A256" s="20"/>
       <c r="B256" s="20"/>
       <c r="C256" s="20" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D256" s="19"/>
       <c r="E256" s="20"/>

</xml_diff>